<commit_message>
potential analysis : LG part
</commit_message>
<xml_diff>
--- a/data/data_collection.xlsx
+++ b/data/data_collection.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8400" tabRatio="719" activeTab="2"/>
+    <workbookView windowWidth="20385" windowHeight="9435" tabRatio="719" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="data11" sheetId="1" r:id="rId1"/>
@@ -673,26 +673,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -709,8 +695,52 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -724,30 +754,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -769,9 +777,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -785,40 +792,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -829,8 +807,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -844,9 +831,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -861,7 +847,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -873,13 +889,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -891,19 +907,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -915,55 +931,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -975,19 +949,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1005,19 +967,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1029,19 +1027,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1052,45 +1038,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1113,7 +1060,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1121,19 +1083,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1152,165 +1118,181 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -3553,6 +3535,55 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
+    <queryTableFields count="10">
+      <queryTableField id="1" dataBound="0"/>
+      <queryTableField id="2" dataBound="0"/>
+      <queryTableField id="3" dataBound="0"/>
+      <queryTableField id="4" dataBound="0"/>
+      <queryTableField id="5" dataBound="0"/>
+      <queryTableField id="6" dataBound="0"/>
+      <queryTableField id="7" dataBound="0"/>
+      <queryTableField id="8" dataBound="0"/>
+      <queryTableField id="9" dataBound="0"/>
+      <queryTableField id="10" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="7">
+    <queryTableFields count="6">
+      <queryTableField id="1" dataBound="0"/>
+      <queryTableField id="2" dataBound="0"/>
+      <queryTableField id="3" dataBound="0"/>
+      <queryTableField id="4" dataBound="0"/>
+      <queryTableField id="5" dataBound="0"/>
+      <queryTableField id="6" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_3" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="7">
+    <queryTableFields count="6">
+      <queryTableField id="1" dataBound="0"/>
+      <queryTableField id="2" dataBound="0"/>
+      <queryTableField id="3" dataBound="0"/>
+      <queryTableField id="4" dataBound="0"/>
+      <queryTableField id="5" dataBound="0"/>
+      <queryTableField id="6" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
     <queryTableFields count="10">
@@ -3571,57 +3602,8 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_3" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="7">
-    <queryTableFields count="6">
-      <queryTableField id="1" dataBound="0"/>
-      <queryTableField id="2" dataBound="0"/>
-      <queryTableField id="3" dataBound="0"/>
-      <queryTableField id="4" dataBound="0"/>
-      <queryTableField id="5" dataBound="0"/>
-      <queryTableField id="6" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="7">
-    <queryTableFields count="6">
-      <queryTableField id="1" dataBound="0"/>
-      <queryTableField id="2" dataBound="0"/>
-      <queryTableField id="3" dataBound="0"/>
-      <queryTableField id="4" dataBound="0"/>
-      <queryTableField id="5" dataBound="0"/>
-      <queryTableField id="6" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
-    <queryTableFields count="10">
-      <queryTableField id="1" dataBound="0"/>
-      <queryTableField id="2" dataBound="0"/>
-      <queryTableField id="3" dataBound="0"/>
-      <queryTableField id="4" dataBound="0"/>
-      <queryTableField id="5" dataBound="0"/>
-      <queryTableField id="6" dataBound="0"/>
-      <queryTableField id="7" dataBound="0"/>
-      <queryTableField id="8" dataBound="0"/>
-      <queryTableField id="9" dataBound="0"/>
-      <queryTableField id="10" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="99-optimized_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="99-optimized" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="11">
     <queryTableFields count="10">
       <queryTableField id="1" dataBound="0"/>
@@ -3640,7 +3622,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="99-optimized" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="99-optimized_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="11">
     <queryTableFields count="10">
       <queryTableField id="1" dataBound="0"/>
@@ -3692,7 +3674,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="10">
     <queryTableFields count="9">
       <queryTableField id="1" dataBound="0"/>
@@ -3710,7 +3692,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="10">
     <queryTableFields count="9">
       <queryTableField id="1" dataBound="0"/>
@@ -5668,10 +5650,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="D15" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="D15" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -5681,6 +5663,7 @@
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="5" width="2.33333333333333" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="12.625"/>
     <col min="10" max="10" width="19.6666666666667" customWidth="1"/>
     <col min="11" max="11" width="4.33333333333333" customWidth="1"/>
     <col min="12" max="15" width="11.5" customWidth="1"/>
@@ -7016,6 +6999,12 @@
       </c>
       <c r="O30">
         <v>24.2393111</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8">
+      <c r="H34">
+        <f>-684.95/3.5^6+3.85^6</f>
+        <v>3256.22708223864</v>
       </c>
     </row>
   </sheetData>
@@ -7041,29 +7030,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="9"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="2:13">
       <c r="B2" s="1">
@@ -7072,11 +7061,11 @@
       <c r="C2">
         <v>-9.35571075</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="6">
         <f>C2+F2</f>
         <v>-9.35571075</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="6">
         <v>0</v>
       </c>
       <c r="F2" s="1">
@@ -7100,11 +7089,11 @@
       <c r="C3">
         <v>-9.36041425</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="6">
         <f t="shared" ref="D3:D18" si="1">C3+F3</f>
         <v>-9.36041425</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="6">
         <v>0</v>
       </c>
       <c r="F3" s="1">
@@ -7113,7 +7102,7 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="7">
         <v>-214.676473994638</v>
       </c>
       <c r="L3">
@@ -7134,11 +7123,11 @@
       <c r="C4">
         <v>-9.36272175</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="6">
         <f t="shared" si="1"/>
         <v>-9.34142444866186</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="6">
         <v>-1.74798</v>
       </c>
       <c r="F4">
@@ -7176,11 +7165,11 @@
       <c r="C5">
         <v>-9.36334625</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="6">
         <f t="shared" si="1"/>
         <v>-9.34203116612822</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="6">
         <v>-1.37949</v>
       </c>
       <c r="F5">
@@ -7215,11 +7204,11 @@
       <c r="C6">
         <v>-9.36387875</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="6">
         <f t="shared" si="1"/>
         <v>-9.34252731341168</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="6">
         <v>-0.649711</v>
       </c>
       <c r="F6">
@@ -7254,11 +7243,11 @@
       <c r="C7">
         <v>-9.364291</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="6">
         <f t="shared" si="1"/>
         <v>-9.34292050564871</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="6">
         <v>-0.436941</v>
       </c>
       <c r="F7">
@@ -7293,11 +7282,11 @@
       <c r="C8">
         <v>-9.36458075</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="6">
         <f t="shared" si="1"/>
         <v>-9.34319526886993</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="6">
         <v>-0.194466</v>
       </c>
       <c r="F8">
@@ -7336,11 +7325,11 @@
       <c r="C9">
         <v>-9.36471925</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="6">
         <f t="shared" si="1"/>
         <v>-9.34329465155856</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="6">
         <v>0.083872</v>
       </c>
       <c r="F9">
@@ -7382,11 +7371,11 @@
       <c r="C10">
         <v>-9.364684</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="6">
         <f t="shared" si="1"/>
         <v>-9.34324236527863</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="6">
         <v>0.40474</v>
       </c>
       <c r="F10">
@@ -7421,11 +7410,11 @@
       <c r="C11">
         <v>-9.36446125</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="6">
         <f t="shared" si="1"/>
         <v>-9.34298510923149</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="6">
         <v>0.766066</v>
       </c>
       <c r="F11">
@@ -7460,11 +7449,11 @@
       <c r="C12">
         <v>-9.36401425</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="6">
         <f t="shared" si="1"/>
         <v>-9.3425189263749</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="6">
         <v>1.209655</v>
       </c>
       <c r="F12">
@@ -7499,11 +7488,11 @@
       <c r="C13">
         <v>-9.363318</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="6">
         <f t="shared" si="1"/>
         <v>-9.34181344827522</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="6">
         <v>1.650845</v>
       </c>
       <c r="F13">
@@ -7538,11 +7527,11 @@
       <c r="C14">
         <v>-9.36232725</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="6">
         <f t="shared" si="1"/>
         <v>-9.34080128378352</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="6">
         <v>2.184954</v>
       </c>
       <c r="F14">
@@ -7584,11 +7573,11 @@
       <c r="C15">
         <v>-9.3610255</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="6">
         <f t="shared" si="1"/>
         <v>-9.33948007495655</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="6">
         <v>2.81936</v>
       </c>
       <c r="F15">
@@ -7630,11 +7619,11 @@
       <c r="C16">
         <v>-9.359363</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="6">
         <f t="shared" si="1"/>
         <v>-9.33780344436616</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="6">
         <v>3.470399</v>
       </c>
       <c r="F16">
@@ -7676,11 +7665,11 @@
       <c r="C17">
         <v>-9.3572985</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="6">
         <f t="shared" si="1"/>
         <v>-9.33572266567675</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="6">
         <v>8.313759</v>
       </c>
       <c r="F17">
@@ -7719,11 +7708,11 @@
       <c r="C18">
         <v>-9.35477725</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="6">
         <f t="shared" si="1"/>
         <v>-9.33318746929334</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="6">
         <v>16.364584</v>
       </c>
       <c r="F18">
@@ -7765,11 +7754,11 @@
       <c r="C19">
         <v>-9.3439195</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="6">
         <f t="shared" ref="D19:D30" si="6">C19+F19</f>
         <v>-9.3439195</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="6">
         <v>29.162834</v>
       </c>
       <c r="F19">
@@ -7804,11 +7793,11 @@
       <c r="C20">
         <v>-9.31057675</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="6">
         <f t="shared" si="6"/>
         <v>-9.31057675</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="6">
         <v>49.590418</v>
       </c>
       <c r="F20">
@@ -7843,11 +7832,11 @@
       <c r="C21">
         <v>-9.2470915</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="6">
         <f t="shared" si="6"/>
         <v>-9.2470915</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="6">
         <v>81.795232</v>
       </c>
       <c r="F21">
@@ -7882,11 +7871,11 @@
       <c r="C22">
         <v>-9.13348925</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="6">
         <f t="shared" si="6"/>
         <v>-9.13348925</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="6">
         <v>126.264436</v>
       </c>
       <c r="F22">
@@ -7921,11 +7910,11 @@
       <c r="C23">
         <v>-8.9380785</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="6">
         <f t="shared" si="6"/>
         <v>-8.9380785</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="6">
         <v>184.537527</v>
       </c>
       <c r="F23">
@@ -7960,11 +7949,11 @@
       <c r="C24">
         <v>-8.63161825</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="6">
         <f t="shared" si="6"/>
         <v>-8.63161825</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="6">
         <v>278.177108</v>
       </c>
       <c r="F24">
@@ -7999,11 +7988,11 @@
       <c r="C25">
         <v>-8.18573275</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="6">
         <f t="shared" si="6"/>
         <v>-8.18573275</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="6">
         <v>410.94174</v>
       </c>
       <c r="F25">
@@ -8038,7 +8027,7 @@
       <c r="C26">
         <v>-7.534209</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="6">
         <f t="shared" si="6"/>
         <v>-7.534209</v>
       </c>
@@ -8063,7 +8052,7 @@
       <c r="C27">
         <v>-6.56529875</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="6">
         <f t="shared" si="6"/>
         <v>-6.56529875</v>
       </c>
@@ -8088,7 +8077,7 @@
       <c r="C28">
         <v>-5.3080285</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="6">
         <f t="shared" si="6"/>
         <v>-5.3080285</v>
       </c>
@@ -8113,7 +8102,7 @@
       <c r="C29">
         <v>-3.53590775</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="6">
         <f t="shared" si="6"/>
         <v>-3.53590775</v>
       </c>
@@ -8135,7 +8124,7 @@
       <c r="C30">
         <v>-9.310968</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="6">
         <f t="shared" si="6"/>
         <v>-9.2921861209303</v>
       </c>
@@ -8177,7 +8166,7 @@
   <sheetPr/>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E16"/>
     </sheetView>
   </sheetViews>
@@ -8229,22 +8218,22 @@
       <c r="C2">
         <v>-1.19325000000003</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="2">
         <v>-0.4985</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2">
         <v>-1.1389</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="2">
         <v>-0.5643</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2">
         <v>-1.1224</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="2">
         <v>-0.5127</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2">
         <v>-1.1448</v>
       </c>
     </row>
@@ -8258,22 +8247,22 @@
       <c r="C3">
         <v>-1.20764865951742</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="2">
         <v>-0.509</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3">
         <v>-1.1675</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="2">
         <v>-0.5759</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3">
         <v>-1.1551</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="2">
         <v>-0.524</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3">
         <v>-1.1717</v>
       </c>
     </row>
@@ -8281,28 +8270,28 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>6.96333826455299</v>
       </c>
       <c r="C4">
         <v>-1.21992613941021</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="2">
         <v>-0.5176</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4">
         <v>-1.1937</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="2">
         <v>-0.586</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4">
         <v>-1.1852</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="2">
         <v>-0.5337</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4">
         <v>-1.1961</v>
       </c>
     </row>
@@ -8310,28 +8299,28 @@
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>6.89702075727153</v>
       </c>
       <c r="C5">
         <v>-1.22943109919572</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="2">
         <v>-0.5239</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5">
         <v>-1.2169</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="2">
         <v>-0.5944</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5">
         <v>-1.2122</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="2">
         <v>-0.5414</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5">
         <v>-1.2175</v>
       </c>
     </row>
@@ -8339,28 +8328,28 @@
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>6.83070324999007</v>
       </c>
       <c r="C6">
         <v>-1.2361116621984</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="2">
         <v>-0.5273</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6">
         <v>-1.2365</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="2">
         <v>-0.6007</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6">
         <v>-1.2352</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="2">
         <v>-0.5467</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6">
         <v>-1.2352</v>
       </c>
     </row>
@@ -8368,28 +8357,28 @@
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>6.76438574270861</v>
       </c>
       <c r="C7">
         <v>-1.23930495978553</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="2">
         <v>-0.527</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7">
         <v>-1.2514</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="2">
         <v>-0.6043</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7">
         <v>-1.2532</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="2">
         <v>-0.5491</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7">
         <v>-1.2484</v>
       </c>
     </row>
@@ -8403,22 +8392,22 @@
       <c r="C8">
         <v>-1.23849222520113</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="2">
         <v>-0.5223</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8">
         <v>-1.2608</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="2">
         <v>-0.6047</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8">
         <v>-1.2652</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="2">
         <v>-0.5479</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8">
         <v>-1.2562</v>
       </c>
     </row>
@@ -8426,28 +8415,28 @@
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>6.6317507281457</v>
       </c>
       <c r="C9">
         <v>-1.23335643431639</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="2">
         <v>-0.5122</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9">
         <v>-1.2636</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="2">
         <v>-0.6014</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9">
         <v>-1.27</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="2">
         <v>-0.5424</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9">
         <v>-1.2576</v>
       </c>
     </row>
@@ -8455,28 +8444,28 @@
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>6.56543322086424</v>
       </c>
       <c r="C10">
         <v>-1.22305026809653</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="2">
         <v>-0.4957</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10">
         <v>-1.2584</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="2">
         <v>-0.5936</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10">
         <v>-1.266</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="2">
         <v>-0.5318</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10">
         <v>-1.2515</v>
       </c>
     </row>
@@ -8484,28 +8473,28 @@
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>6.49911571358279</v>
       </c>
       <c r="C11">
         <v>-1.20699731903488</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="2">
         <v>-0.4715</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11">
         <v>-1.2439</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="2">
         <v>-0.5804</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11">
         <v>-1.2516</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="2">
         <v>-0.5151</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11">
         <v>-1.2365</v>
       </c>
     </row>
@@ -8513,28 +8502,28 @@
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>6.43279820630133</v>
       </c>
       <c r="C12">
         <v>-1.18415428954427</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="2">
         <v>-0.4379</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12">
         <v>-1.2182</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="2">
         <v>-0.5609</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12">
         <v>-1.2247</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="2">
         <v>-0.4912</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12">
         <v>-1.2112</v>
       </c>
     </row>
@@ -8542,28 +8531,28 @@
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>6.36648069901987</v>
       </c>
       <c r="C13">
         <v>-1.15414075067028</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="2">
         <v>-0.3934</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13">
         <v>-1.1796</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="2">
         <v>-0.534</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13">
         <v>-1.1832</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="2">
         <v>-0.4588</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13">
         <v>-1.1738</v>
       </c>
     </row>
@@ -8571,28 +8560,28 @@
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="6">
         <v>6.30016319173841</v>
       </c>
       <c r="C14">
         <v>-1.11580965147456</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="2">
         <v>-0.3357</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14">
         <v>-1.1258</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="2">
         <v>-0.4983</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14">
         <v>-1.1243</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="2">
         <v>-0.4165</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14">
         <v>-1.1224</v>
       </c>
     </row>
@@ -8606,22 +8595,22 @@
       <c r="C15">
         <v>-1.06820991957107</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="2">
         <v>-0.2625</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15">
         <v>-1.0542</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="2">
         <v>-0.4524</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15">
         <v>-1.0449</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="2">
         <v>-0.3625</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15">
         <v>-1.0548</v>
       </c>
     </row>
@@ -8635,22 +8624,22 @@
       <c r="C16">
         <v>-1.01007922252012</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="2">
         <v>-0.171</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16">
         <v>-0.9622</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="2">
         <v>-0.3943</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16">
         <v>-0.9414</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="2">
         <v>-0.2949</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16">
         <v>-0.9687</v>
       </c>
     </row>
@@ -8717,7 +8706,6 @@
       <c r="I1" t="s">
         <v>50</v>
       </c>
-      <c r="J1"/>
       <c r="L1" t="s">
         <v>51</v>
       </c>
@@ -8751,12 +8739,7 @@
     </row>
     <row r="2" spans="4:21">
       <c r="D2" s="2"/>
-      <c r="E2"/>
       <c r="F2" s="2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
       <c r="L2" t="s">
         <v>51</v>
       </c>
@@ -8940,7 +8923,6 @@
       <c r="I5" t="s">
         <v>57</v>
       </c>
-      <c r="J5"/>
       <c r="L5" t="s">
         <v>51</v>
       </c>
@@ -9000,7 +8982,6 @@
       <c r="I6" t="s">
         <v>59</v>
       </c>
-      <c r="J6"/>
       <c r="L6" t="s">
         <v>51</v>
       </c>
@@ -9060,7 +9041,6 @@
       <c r="I7" t="s">
         <v>61</v>
       </c>
-      <c r="J7"/>
       <c r="L7" t="s">
         <v>51</v>
       </c>
@@ -9120,7 +9100,6 @@
       <c r="I8" t="s">
         <v>63</v>
       </c>
-      <c r="J8"/>
       <c r="L8" t="s">
         <v>51</v>
       </c>
@@ -9180,7 +9159,6 @@
       <c r="I9" t="s">
         <v>65</v>
       </c>
-      <c r="J9"/>
       <c r="L9" t="s">
         <v>51</v>
       </c>
@@ -9240,7 +9218,6 @@
       <c r="I10" t="s">
         <v>67</v>
       </c>
-      <c r="J10"/>
       <c r="L10" t="s">
         <v>51</v>
       </c>
@@ -9300,7 +9277,6 @@
       <c r="I11" t="s">
         <v>69</v>
       </c>
-      <c r="J11"/>
       <c r="L11" t="s">
         <v>51</v>
       </c>
@@ -9360,7 +9336,6 @@
       <c r="I12" t="s">
         <v>71</v>
       </c>
-      <c r="J12"/>
       <c r="L12" t="s">
         <v>51</v>
       </c>
@@ -9420,7 +9395,6 @@
       <c r="I13" t="s">
         <v>73</v>
       </c>
-      <c r="J13"/>
       <c r="L13" t="s">
         <v>51</v>
       </c>
@@ -9480,7 +9454,6 @@
       <c r="I14" t="s">
         <v>75</v>
       </c>
-      <c r="J14"/>
       <c r="L14" t="s">
         <v>51</v>
       </c>
@@ -9540,7 +9513,6 @@
       <c r="I15" t="s">
         <v>77</v>
       </c>
-      <c r="J15"/>
       <c r="L15" t="s">
         <v>51</v>
       </c>
@@ -9632,37 +9604,30 @@
     </row>
     <row r="18" spans="4:6">
       <c r="D18" s="2"/>
-      <c r="E18"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="4:6">
       <c r="D19" s="2"/>
-      <c r="E19"/>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="4:6">
       <c r="D20" s="2"/>
-      <c r="E20"/>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="4:6">
       <c r="D21" s="2"/>
-      <c r="E21"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="4:6">
       <c r="D22" s="2"/>
-      <c r="E22"/>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="4:6">
       <c r="D23" s="2"/>
-      <c r="E23"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="4:6">
       <c r="D24" s="2"/>
-      <c r="E24"/>
       <c r="F24" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct trainset.in in MD-X6 potential
</commit_message>
<xml_diff>
--- a/data/data_collection.xlsx
+++ b/data/data_collection.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="719" activeTab="7"/>
+    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="719" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data11" sheetId="1" r:id="rId1"/>
@@ -720,8 +720,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -734,9 +734,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -744,35 +743,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -794,9 +764,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -809,9 +794,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -825,16 +816,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -848,8 +832,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -864,14 +872,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -879,7 +879,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -894,31 +894,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -930,13 +924,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -948,19 +984,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -978,7 +1008,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -990,19 +1020,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1014,13 +1038,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1032,49 +1074,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1085,15 +1085,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1131,6 +1122,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1160,21 +1166,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1185,151 +1176,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4727,8 +4727,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
     </queryTableFields>
@@ -4737,7 +4737,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="10">
     <queryTableFields count="9">
       <queryTableField id="1" dataBound="0"/>
@@ -4755,7 +4755,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="10">
     <queryTableFields count="9">
       <queryTableField id="1" dataBound="0"/>
@@ -4791,7 +4791,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="7">
     <queryTableFields count="6">
       <queryTableField id="1" dataBound="0"/>
@@ -4806,7 +4806,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="7">
     <queryTableFields count="6">
       <queryTableField id="1" dataBound="0"/>
@@ -4831,8 +4831,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
     </queryTableFields>
@@ -4841,6 +4841,25 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
+    <queryTableFields count="10">
+      <queryTableField id="1" dataBound="0"/>
+      <queryTableField id="2" dataBound="0"/>
+      <queryTableField id="3" dataBound="0"/>
+      <queryTableField id="4" dataBound="0"/>
+      <queryTableField id="5" dataBound="0"/>
+      <queryTableField id="6" dataBound="0"/>
+      <queryTableField id="7" dataBound="0"/>
+      <queryTableField id="8" dataBound="0"/>
+      <queryTableField id="9" dataBound="0"/>
+      <queryTableField id="10" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
     <queryTableFields count="10">
@@ -4859,27 +4878,8 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
-    <queryTableFields count="10">
-      <queryTableField id="1" dataBound="0"/>
-      <queryTableField id="2" dataBound="0"/>
-      <queryTableField id="3" dataBound="0"/>
-      <queryTableField id="4" dataBound="0"/>
-      <queryTableField id="5" dataBound="0"/>
-      <queryTableField id="6" dataBound="0"/>
-      <queryTableField id="7" dataBound="0"/>
-      <queryTableField id="8" dataBound="0"/>
-      <queryTableField id="9" dataBound="0"/>
-      <queryTableField id="10" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
     <queryTableFields count="10">
       <queryTableField id="1" dataBound="0"/>
@@ -4898,7 +4898,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
     <queryTableFields count="10">
       <queryTableField id="1" dataBound="0"/>
@@ -8237,8 +8237,8 @@
   <sheetPr/>
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -8249,7 +8249,9 @@
     <col min="5" max="5" width="11.5"/>
     <col min="6" max="6" width="12.625"/>
     <col min="7" max="7" width="21.8333333333333" customWidth="1"/>
-    <col min="8" max="11" width="14.1666666666667" customWidth="1"/>
+    <col min="8" max="9" width="14.1666666666667" customWidth="1"/>
+    <col min="10" max="10" width="20.375" customWidth="1"/>
+    <col min="11" max="11" width="14.1666666666667" customWidth="1"/>
     <col min="12" max="13" width="12.625"/>
     <col min="15" max="15" width="12.625"/>
   </cols>
@@ -62212,7 +62214,7 @@
   <sheetPr/>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
correct shift data for QM+phn
</commit_message>
<xml_diff>
--- a/data/data_collection.xlsx
+++ b/data/data_collection.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7950" tabRatio="719" activeTab="4"/>
+    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="719" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="data11" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <definedName name="ExternalData_1" localSheetId="2">CCmd!$K$2:$K$16</definedName>
     <definedName name="ExternalData_3" localSheetId="2">CCmd!$J$2:$J$16</definedName>
     <definedName name="ExternalData_4" localSheetId="2">CCmd!$M$2:$M$16</definedName>
-    <definedName name="ExternalData_1" localSheetId="7">Sheet6!$A$1:$A$15</definedName>
+    <definedName name="ExternalData_1" localSheetId="7">Sheet6!$B$1:$B$15</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -779,12 +779,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0.00000"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="179" formatCode="0.00000"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -796,9 +797,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -810,8 +832,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -820,6 +843,90 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -839,112 +946,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -955,7 +956,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -967,25 +992,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -997,31 +1052,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1033,13 +1064,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1051,13 +1094,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1069,49 +1118,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1129,13 +1136,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1149,11 +1150,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1175,50 +1206,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1246,155 +1236,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1404,22 +1405,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4752,7 +4745,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -4812,6 +4805,21 @@
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_3" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="7">
+    <queryTableFields count="6">
+      <queryTableField id="1" dataBound="0"/>
+      <queryTableField id="2" dataBound="0"/>
+      <queryTableField id="3" dataBound="0"/>
+      <queryTableField id="4" dataBound="0"/>
+      <queryTableField id="5" dataBound="0"/>
+      <queryTableField id="6" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="7">
     <queryTableFields count="6">
@@ -4826,22 +4834,17 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_3" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="7">
-    <queryTableFields count="6">
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_4" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
+    <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
-      <queryTableField id="2" dataBound="0"/>
-      <queryTableField id="3" dataBound="0"/>
-      <queryTableField id="4" dataBound="0"/>
-      <queryTableField id="5" dataBound="0"/>
-      <queryTableField id="6" dataBound="0"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
@@ -4851,18 +4854,8 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_4" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -4882,6 +4875,25 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
+    <queryTableFields count="10">
+      <queryTableField id="1" dataBound="0"/>
+      <queryTableField id="2" dataBound="0"/>
+      <queryTableField id="3" dataBound="0"/>
+      <queryTableField id="4" dataBound="0"/>
+      <queryTableField id="5" dataBound="0"/>
+      <queryTableField id="6" dataBound="0"/>
+      <queryTableField id="7" dataBound="0"/>
+      <queryTableField id="8" dataBound="0"/>
+      <queryTableField id="9" dataBound="0"/>
+      <queryTableField id="10" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
     <queryTableFields count="10">
@@ -4900,27 +4912,8 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
-    <queryTableFields count="10">
-      <queryTableField id="1" dataBound="0"/>
-      <queryTableField id="2" dataBound="0"/>
-      <queryTableField id="3" dataBound="0"/>
-      <queryTableField id="4" dataBound="0"/>
-      <queryTableField id="5" dataBound="0"/>
-      <queryTableField id="6" dataBound="0"/>
-      <queryTableField id="7" dataBound="0"/>
-      <queryTableField id="8" dataBound="0"/>
-      <queryTableField id="9" dataBound="0"/>
-      <queryTableField id="10" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
     <queryTableFields count="10">
       <queryTableField id="1" dataBound="0"/>
@@ -4939,7 +4932,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
     <queryTableFields count="10">
       <queryTableField id="1" dataBound="0"/>
@@ -10453,7 +10446,7 @@
   <sheetPr/>
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D3" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -10509,11 +10502,11 @@
       <c r="B2" s="1">
         <v>7.62651333736756</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="12">
         <f>C2+F2</f>
         <v>0</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="12">
         <v>0</v>
       </c>
       <c r="F2" s="1">
@@ -10534,11 +10527,11 @@
       <c r="B3" s="1">
         <v>7.29492580096027</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="12">
         <f>C3+F3</f>
         <v>0</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="12">
         <v>0</v>
       </c>
       <c r="F3" s="1">
@@ -10571,10 +10564,10 @@
       <c r="C4">
         <v>-9.3677675</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="12">
         <v>-9.34698083397609</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="12">
         <v>-1.74798</v>
       </c>
       <c r="F4">
@@ -10620,10 +10613,10 @@
       <c r="C5">
         <v>-9.368439</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <v>-9.34744931354813</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="12">
         <v>-1.37949</v>
       </c>
       <c r="F5">
@@ -10666,10 +10659,10 @@
       <c r="C6">
         <v>-9.36901625</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <v>-9.34794841229954</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="12">
         <v>-0.649711</v>
       </c>
       <c r="F6">
@@ -10712,10 +10705,10 @@
       <c r="C7">
         <v>-9.3694765</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <v>-9.34833158156986</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="12">
         <v>-0.436941</v>
       </c>
       <c r="F7">
@@ -10758,10 +10751,10 @@
       <c r="C8">
         <v>-9.3698085</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="12">
         <v>-9.34862086397872</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="12">
         <v>-0.194466</v>
       </c>
       <c r="F8">
@@ -10808,10 +10801,10 @@
       <c r="C9">
         <v>-9.36999225</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="12">
         <v>-9.34876171862637</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="12">
         <v>0.083872</v>
       </c>
       <c r="F9">
@@ -10861,10 +10854,10 @@
       <c r="C10">
         <v>-9.3700015</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="12">
         <v>-9.34872362538945</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="12">
         <v>0.40474</v>
       </c>
       <c r="F10">
@@ -10907,10 +10900,10 @@
       <c r="C11">
         <v>-9.36981575</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="12">
         <v>-9.34850205543826</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="12">
         <v>0.766066</v>
       </c>
       <c r="F11">
@@ -10953,10 +10946,10 @@
       <c r="C12">
         <v>-9.3694085</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <v>-9.34806046626898</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="12">
         <v>1.209655</v>
       </c>
       <c r="F12">
@@ -10999,10 +10992,10 @@
       <c r="C13">
         <v>-9.36874575</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="12">
         <v>-9.34736732532241</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="12">
         <v>1.650845</v>
       </c>
       <c r="F13">
@@ -11045,10 +11038,10 @@
       <c r="C14">
         <v>-9.36779125</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="12">
         <v>-9.34638814932725</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="12">
         <v>2.184954</v>
       </c>
       <c r="F14">
@@ -11098,10 +11091,10 @@
       <c r="C15">
         <v>-9.3665155</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="12">
         <v>-9.34508736923487</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="12">
         <v>2.81936</v>
       </c>
       <c r="F15">
@@ -11151,10 +11144,10 @@
       <c r="C16">
         <v>-9.3648825</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="12">
         <v>-9.34343159581578</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="12">
         <v>3.470399</v>
       </c>
       <c r="F16">
@@ -11204,10 +11197,10 @@
       <c r="C17">
         <v>-9.36283875</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="12">
         <v>-9.34136838860836</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="12">
         <v>8.313759</v>
       </c>
       <c r="F17">
@@ -11254,10 +11247,10 @@
       <c r="C18">
         <v>-9.360343</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="12">
         <v>-9.33885459866432</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="12">
         <v>16.364584</v>
       </c>
       <c r="F18">
@@ -11298,8 +11291,8 @@
       </c>
     </row>
     <row r="19" spans="4:5">
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
@@ -11311,11 +11304,11 @@
       <c r="C20">
         <v>-9.3439195</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="12">
         <f t="shared" ref="D20:D31" si="7">C20+F20</f>
         <v>-9.3439195</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="12">
         <v>29.162834</v>
       </c>
       <c r="F20">
@@ -11350,11 +11343,11 @@
       <c r="C21">
         <v>-9.31057675</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="12">
         <f t="shared" si="7"/>
         <v>-9.31057675</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="12">
         <v>49.590418</v>
       </c>
       <c r="F21">
@@ -11389,11 +11382,11 @@
       <c r="C22">
         <v>-9.2470915</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="12">
         <f t="shared" si="7"/>
         <v>-9.2470915</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="12">
         <v>81.795232</v>
       </c>
       <c r="F22">
@@ -11428,11 +11421,11 @@
       <c r="C23">
         <v>-9.13348925</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="12">
         <f t="shared" si="7"/>
         <v>-9.13348925</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="12">
         <v>126.264436</v>
       </c>
       <c r="F23">
@@ -11467,11 +11460,11 @@
       <c r="C24">
         <v>-8.9380785</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="12">
         <f t="shared" si="7"/>
         <v>-8.9380785</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="12">
         <v>184.537527</v>
       </c>
       <c r="F24">
@@ -11506,11 +11499,11 @@
       <c r="C25">
         <v>-8.63161825</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="12">
         <f t="shared" si="7"/>
         <v>-8.63161825</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="12">
         <v>278.177108</v>
       </c>
       <c r="F25">
@@ -11545,11 +11538,11 @@
       <c r="C26">
         <v>-8.18573275</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="12">
         <f t="shared" si="7"/>
         <v>-8.18573275</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="12">
         <v>410.94174</v>
       </c>
       <c r="F26">
@@ -11584,7 +11577,7 @@
       <c r="C27">
         <v>-7.534209</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="12">
         <f t="shared" si="7"/>
         <v>-7.534209</v>
       </c>
@@ -11609,7 +11602,7 @@
       <c r="C28">
         <v>-6.56529875</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="12">
         <f t="shared" si="7"/>
         <v>-6.56529875</v>
       </c>
@@ -11634,7 +11627,7 @@
       <c r="C29">
         <v>-5.3080285</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="12">
         <f t="shared" si="7"/>
         <v>-5.3080285</v>
       </c>
@@ -11659,7 +11652,7 @@
       <c r="C30">
         <v>-3.53590775</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="12">
         <f t="shared" si="7"/>
         <v>-3.53590775</v>
       </c>
@@ -11681,7 +11674,7 @@
       <c r="C31" s="2">
         <v>-9.315113</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="12">
         <f t="shared" si="7"/>
         <v>-9.29649673814039</v>
       </c>
@@ -11729,7 +11722,7 @@
   <dimension ref="A1:M16381"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -11749,8 +11742,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -11783,12 +11776,12 @@
       <c r="L1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4">
@@ -11800,19 +11793,19 @@
       <c r="D2">
         <v>-1.16397647235087</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>-0.4985</v>
       </c>
       <c r="F2" s="4">
         <v>-1.1389</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>-0.5643</v>
       </c>
       <c r="H2" s="4">
         <v>-1.1224</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="10">
         <v>-0.5127</v>
       </c>
       <c r="J2">
@@ -11821,7 +11814,7 @@
       <c r="K2">
         <v>-1.1354</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="11">
         <v>-1.1812</v>
       </c>
       <c r="M2">
@@ -11829,7 +11822,7 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4">
@@ -11841,19 +11834,19 @@
       <c r="D3">
         <v>-1.17477787803332</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <v>-0.509</v>
       </c>
       <c r="F3" s="4">
         <v>-1.1675</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <v>-0.5759</v>
       </c>
       <c r="H3" s="4">
         <v>-1.1551</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="10">
         <v>-0.524</v>
       </c>
       <c r="J3">
@@ -11862,7 +11855,7 @@
       <c r="K3">
         <v>-1.1552</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="11">
         <v>-1.2007</v>
       </c>
       <c r="M3">
@@ -11870,10 +11863,10 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="6">
         <v>6.96333826455299</v>
       </c>
       <c r="C4" s="4">
@@ -11882,19 +11875,19 @@
       <c r="D4">
         <v>-1.18628524870925</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>-0.5176</v>
       </c>
       <c r="F4" s="4">
         <v>-1.1937</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <v>-0.586</v>
       </c>
       <c r="H4" s="4">
         <v>-1.1852</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="10">
         <v>-0.5337</v>
       </c>
       <c r="J4">
@@ -11903,7 +11896,7 @@
       <c r="K4">
         <v>-1.1726</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="11">
         <v>-1.2173</v>
       </c>
       <c r="M4">
@@ -11911,10 +11904,10 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="6">
         <v>6.89702075727153</v>
       </c>
       <c r="C5" s="4">
@@ -11923,19 +11916,19 @@
       <c r="D5">
         <v>-1.19511971445925</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>-0.5239</v>
       </c>
       <c r="F5" s="4">
         <v>-1.2169</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>-0.5944</v>
       </c>
       <c r="H5" s="4">
         <v>-1.2122</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <v>-0.5414</v>
       </c>
       <c r="J5">
@@ -11944,7 +11937,7 @@
       <c r="K5">
         <v>-1.1872</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="11">
         <v>-1.2304</v>
       </c>
       <c r="M5">
@@ -11952,10 +11945,10 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="6">
         <v>6.83070324999007</v>
       </c>
       <c r="C6" s="4">
@@ -11964,19 +11957,19 @@
       <c r="D6">
         <v>-1.20178949654021</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>-0.5273</v>
       </c>
       <c r="F6" s="4">
         <v>-1.2365</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <v>-0.6007</v>
       </c>
       <c r="H6" s="4">
         <v>-1.2352</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <v>-0.5467</v>
       </c>
       <c r="J6">
@@ -11985,7 +11978,7 @@
       <c r="K6">
         <v>-1.1983</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="11">
         <v>-1.2394</v>
       </c>
       <c r="M6">
@@ -11993,10 +11986,10 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="6">
         <v>6.76438574270861</v>
       </c>
       <c r="C7" s="4">
@@ -12005,19 +11998,19 @@
       <c r="D7">
         <v>-1.20503708359058</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>-0.527</v>
       </c>
       <c r="F7" s="4">
         <v>-1.2514</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>-0.6043</v>
       </c>
       <c r="H7" s="4">
         <v>-1.2532</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="10">
         <v>-0.5491</v>
       </c>
       <c r="J7">
@@ -12026,7 +12019,7 @@
       <c r="K7">
         <v>-1.2055</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="11">
         <v>-1.2435</v>
       </c>
       <c r="M7">
@@ -12034,7 +12027,7 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="4">
@@ -12046,19 +12039,19 @@
       <c r="D8">
         <v>-1.20415879448197</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>-0.5223</v>
       </c>
       <c r="F8" s="4">
         <v>-1.2608</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <v>-0.6047</v>
       </c>
       <c r="H8" s="4">
         <v>-1.2652</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <v>-0.5479</v>
       </c>
       <c r="J8">
@@ -12067,7 +12060,7 @@
       <c r="K8">
         <v>-1.208</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="11">
         <v>-1.2419</v>
       </c>
       <c r="M8">
@@ -12075,10 +12068,10 @@
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="6">
         <v>6.6317507281457</v>
       </c>
       <c r="C9" s="4">
@@ -12087,19 +12080,19 @@
       <c r="D9">
         <v>-1.19905021115693</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>-0.5122</v>
       </c>
       <c r="F9" s="4">
         <v>-1.2636</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="10">
         <v>-0.6014</v>
       </c>
       <c r="H9" s="4">
         <v>-1.27</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>-0.5424</v>
       </c>
       <c r="J9">
@@ -12108,7 +12101,7 @@
       <c r="K9">
         <v>-1.2051</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="11">
         <v>-1.2337</v>
       </c>
       <c r="M9">
@@ -12116,10 +12109,10 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="6">
         <v>6.56543322086424</v>
       </c>
       <c r="C10" s="4">
@@ -12128,19 +12121,19 @@
       <c r="D10">
         <v>-1.18886879867486</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>-0.4957</v>
       </c>
       <c r="F10" s="4">
         <v>-1.2584</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <v>-0.5936</v>
       </c>
       <c r="H10" s="4">
         <v>-1.266</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <v>-0.5318</v>
       </c>
       <c r="J10">
@@ -12149,7 +12142,7 @@
       <c r="K10">
         <v>-1.1959</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="11">
         <v>-1.2176</v>
       </c>
       <c r="M10">
@@ -12157,10 +12150,10 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="6">
         <v>6.49911571358279</v>
       </c>
       <c r="C11" s="4">
@@ -12169,19 +12162,19 @@
       <c r="D11">
         <v>-1.17288753288264</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>-0.4715</v>
       </c>
       <c r="F11" s="4">
         <v>-1.2439</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <v>-0.5804</v>
       </c>
       <c r="H11" s="4">
         <v>-1.2516</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>-0.5151</v>
       </c>
       <c r="J11">
@@ -12190,7 +12183,7 @@
       <c r="K11">
         <v>-1.1794</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="11">
         <v>-1.1925</v>
       </c>
       <c r="M11">
@@ -12198,10 +12191,10 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="6">
         <v>6.43279820630133</v>
       </c>
       <c r="C12" s="4">
@@ -12210,19 +12203,19 @@
       <c r="D12">
         <v>-1.15031135712294</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>-0.4379</v>
       </c>
       <c r="F12" s="4">
         <v>-1.2182</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="10">
         <v>-0.5609</v>
       </c>
       <c r="H12" s="4">
         <v>-1.2247</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="10">
         <v>-0.4912</v>
       </c>
       <c r="J12">
@@ -12231,7 +12224,7 @@
       <c r="K12">
         <v>-1.1545</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="11">
         <v>-1.1569</v>
       </c>
       <c r="M12">
@@ -12239,10 +12232,10 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="6">
         <v>6.36648069901987</v>
       </c>
       <c r="C13" s="4">
@@ -12251,19 +12244,19 @@
       <c r="D13">
         <v>-1.12032018073023</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>-0.3934</v>
       </c>
       <c r="F13" s="4">
         <v>-1.1796</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="10">
         <v>-0.534</v>
       </c>
       <c r="H13" s="4">
         <v>-1.1832</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="10">
         <v>-0.4588</v>
       </c>
       <c r="J13">
@@ -12272,7 +12265,7 @@
       <c r="K13">
         <v>-1.1198</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="11">
         <v>-1.1092</v>
       </c>
       <c r="M13">
@@ -12280,10 +12273,10 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="6">
         <v>6.30016319173841</v>
       </c>
       <c r="C14" s="4">
@@ -12292,19 +12285,19 @@
       <c r="D14">
         <v>-1.08214417160377</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <v>-0.3357</v>
       </c>
       <c r="F14" s="4">
         <v>-1.1258</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="10">
         <v>-0.4983</v>
       </c>
       <c r="H14" s="4">
         <v>-1.1243</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="10">
         <v>-0.4165</v>
       </c>
       <c r="J14">
@@ -12313,7 +12306,7 @@
       <c r="K14">
         <v>-1.0741</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="11">
         <v>-1.0475</v>
       </c>
       <c r="M14">
@@ -12321,7 +12314,7 @@
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4">
@@ -12333,19 +12326,19 @@
       <c r="D15">
         <v>-1.03457424671424</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>-0.2625</v>
       </c>
       <c r="F15" s="4">
         <v>-1.0542</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="10">
         <v>-0.4524</v>
       </c>
       <c r="H15" s="4">
         <v>-1.0449</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="10">
         <v>-0.3625</v>
       </c>
       <c r="J15">
@@ -12354,7 +12347,7 @@
       <c r="K15">
         <v>-1.0156</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="11">
         <v>-0.9697</v>
       </c>
       <c r="M15">
@@ -12362,7 +12355,7 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="4">
@@ -12374,19 +12367,19 @@
       <c r="D16">
         <v>-0.976615550953454</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>-0.171</v>
       </c>
       <c r="F16" s="4">
         <v>-0.9622</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="10">
         <v>-0.3943</v>
       </c>
       <c r="H16" s="4">
         <v>-0.9414</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <v>-0.2949</v>
       </c>
       <c r="J16">
@@ -12395,7 +12388,7 @@
       <c r="K16">
         <v>-0.9425</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="11">
         <v>-0.8734</v>
       </c>
       <c r="M16">
@@ -62118,8 +62111,8 @@
   <sheetPr/>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -62482,7 +62475,7 @@
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>7.0959732791159</v>
       </c>
       <c r="C2">
@@ -62499,7 +62492,7 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>7.02965577183444</v>
       </c>
       <c r="C3">
@@ -62584,7 +62577,7 @@
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>6.69806823542716</v>
       </c>
       <c r="C8">
@@ -62703,7 +62696,7 @@
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>6.23384568445696</v>
       </c>
       <c r="C15">
@@ -62720,7 +62713,7 @@
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>6.1675281771755</v>
       </c>
       <c r="C16">
@@ -62769,7 +62762,7 @@
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>7.0959732791159</v>
       </c>
       <c r="C2">
@@ -62786,7 +62779,7 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>7.02965577183444</v>
       </c>
       <c r="C3">
@@ -62871,7 +62864,7 @@
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>6.69806823542716</v>
       </c>
       <c r="C8">
@@ -62990,7 +62983,7 @@
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>6.23384568445696</v>
       </c>
       <c r="C15">
@@ -63007,7 +63000,7 @@
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>6.1675281771755</v>
       </c>
       <c r="C16">
@@ -63029,90 +63022,196 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="8.375" customWidth="1"/>
+    <col min="2" max="3" width="19.875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1">
-        <v>-1.1174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2">
-        <v>-1.1415</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
-        <v>-1.163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
-        <v>-1.1814</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5">
-        <v>-1.1961</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6">
-        <v>-1.2063</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7">
-        <v>-1.2112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8">
-        <v>-1.2099</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9">
-        <v>-1.2013</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10">
-        <v>-1.1843</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11">
-        <v>-1.1575</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12">
-        <v>-1.1193</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13">
-        <v>-1.0682</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14">
-        <v>-1.0022</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15">
-        <v>-0.9191</v>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4">
+        <v>7.0959732791159</v>
+      </c>
+      <c r="C1" s="5">
+        <f>B1-0.0733</f>
+        <v>7.0226732791159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>7.02965577183444</v>
+      </c>
+      <c r="C2" s="5">
+        <f t="shared" ref="C2:C15" si="0">B2-0.0733</f>
+        <v>6.95635577183444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <v>6.96333826455299</v>
+      </c>
+      <c r="C3" s="5">
+        <f t="shared" si="0"/>
+        <v>6.89003826455299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>6.89702075727153</v>
+      </c>
+      <c r="C4" s="5">
+        <f t="shared" si="0"/>
+        <v>6.82372075727153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>6.83070324999007</v>
+      </c>
+      <c r="C5" s="5">
+        <f t="shared" si="0"/>
+        <v>6.75740324999007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6">
+        <v>6.76438574270861</v>
+      </c>
+      <c r="C6" s="5">
+        <f t="shared" si="0"/>
+        <v>6.69108574270861</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6.69806823542716</v>
+      </c>
+      <c r="C7" s="5">
+        <f t="shared" si="0"/>
+        <v>6.62476823542716</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6">
+        <v>6.6317507281457</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" si="0"/>
+        <v>6.5584507281457</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6">
+        <v>6.56543322086424</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" si="0"/>
+        <v>6.49213322086424</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6">
+        <v>6.49911571358279</v>
+      </c>
+      <c r="C10" s="5">
+        <f t="shared" si="0"/>
+        <v>6.42581571358279</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6">
+        <v>6.43279820630133</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="0"/>
+        <v>6.35949820630133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="6">
+        <v>6.36648069901987</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="0"/>
+        <v>6.29318069901987</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="6">
+        <v>6.30016319173841</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" si="0"/>
+        <v>6.22686319173841</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4">
+        <v>6.23384568445696</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="0"/>
+        <v>6.16054568445696</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="4">
+        <v>6.1675281771755</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="0"/>
+        <v>6.0942281771755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>